<commit_message>
running if jar made from ij but not from mvn
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/new_customers.xlsx
+++ b/src/test/resources/testData/new_customers.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>dob</t>
   </si>
@@ -84,33 +84,9 @@
     <t>SelectorType</t>
   </si>
   <si>
-    <t>field type</t>
-  </si>
-  <si>
     <t>whatever</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>css</t>
-  </si>
-  <si>
-    <t>selector</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>radioButton</t>
-  </si>
-  <si>
-    <t>checkbox</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -133,13 +109,28 @@
   </si>
   <si>
     <t>file:///Users/44022649/fc572/pagefiller/src/test/resources/testData/pageTwo.html</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Click me</t>
+  </si>
+  <si>
+    <t>Element Name</t>
+  </si>
+  <si>
+    <t>Element Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +142,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,11 +174,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,124 +476,130 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>32</v>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="file:///src/test/resources/testData/pageOne.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="69" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
@@ -606,8 +612,8 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -621,7 +627,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -635,90 +641,88 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -732,18 +736,8 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>